<commit_message>
word to excel new worksheet
</commit_message>
<xml_diff>
--- a/Twitter.UI/AdminExcel.xlsx
+++ b/Twitter.UI/AdminExcel.xlsx
@@ -5,16 +5,15 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Worksheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Worksheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Monthly Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Users Report" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Tarih</t>
   </si>
@@ -46,7 +45,73 @@
     <t>08/2023</t>
   </si>
   <si>
+    <t>ysfsck</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Takip Edilen</t>
+  </si>
+  <si>
+    <t>Takipçi</t>
+  </si>
+  <si>
+    <t>Bu Ay Atılan Tweetler</t>
+  </si>
+  <si>
+    <t>Etkileşim</t>
+  </si>
+  <si>
+    <t>fatma19</t>
+  </si>
+  <si>
+    <t>ruyaa</t>
+  </si>
+  <si>
     <t>gizemm3</t>
+  </si>
+  <si>
+    <t>nilaysu_</t>
+  </si>
+  <si>
+    <t>davidturner</t>
+  </si>
+  <si>
+    <t>selin6</t>
+  </si>
+  <si>
+    <t>melisaa18</t>
+  </si>
+  <si>
+    <t>irem</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>kerem18</t>
+  </si>
+  <si>
+    <t>simge</t>
+  </si>
+  <si>
+    <t>mert</t>
+  </si>
+  <si>
+    <t>azraa</t>
+  </si>
+  <si>
+    <t>ipekk</t>
+  </si>
+  <si>
+    <t>ece</t>
+  </si>
+  <si>
+    <t>ranas</t>
+  </si>
+  <si>
+    <t>duyguu</t>
   </si>
 </sst>
 </file>
@@ -176,7 +241,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -186,22 +251,381 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.584197998046875" customWidth="1"/>
+    <col min="2" max="2" width="14.71049976348877" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.033416748046875" customWidth="1"/>
+    <col min="5" max="5" width="25.68185043334961" customWidth="1"/>
+    <col min="6" max="6" width="11.23523998260498" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0">
+        <v>3</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0">
+        <v>3</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="0">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="0">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0">
+        <v>2</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0">
+        <v>2</v>
+      </c>
+      <c r="E12" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="0">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="0">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="0">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="0">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0">
+        <v>2</v>
+      </c>
+      <c r="E17" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="0">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="0">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0</v>
+      </c>
+      <c r="C20" s="0">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0</v>
+      </c>
+      <c r="C21" s="0">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>